<commit_message>
Complete all the code part. TODO: xml part
</commit_message>
<xml_diff>
--- a/翻译规范.xlsx
+++ b/翻译规范.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="200">
   <si>
     <t>中</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -357,6 +357,515 @@
   </si>
   <si>
     <t>必须大于等于-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张海羊</t>
+  </si>
+  <si>
+    <t>Alice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘婧</t>
+  </si>
+  <si>
+    <t>Bob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王锋</t>
+  </si>
+  <si>
+    <t>Cathy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先选择识别引擎类型</t>
+  </si>
+  <si>
+    <t>Please select the recognition engine type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>上传预设关键词</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="Lucida Sans Typewriter"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>语法文件</t>
+    </r>
+  </si>
+  <si>
+    <t>Upload pre-defined keyword / grammar file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语法构建失败</t>
+  </si>
+  <si>
+    <t>Grammar build failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>错误码</t>
+  </si>
+  <si>
+    <t>error code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新词典失败</t>
+  </si>
+  <si>
+    <t>Update dictionary failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请先构建语法</t>
+  </si>
+  <si>
+    <t>Please build grammar first</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>识别失败</t>
+  </si>
+  <si>
+    <t>Recognition failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>停止识别</t>
+  </si>
+  <si>
+    <t>Stop recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消识别</t>
+  </si>
+  <si>
+    <t>Cancel recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始化失败</t>
+  </si>
+  <si>
+    <t>Initialization failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>词典更新成功</t>
+  </si>
+  <si>
+    <t>Dictionary update succeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>词典更新失败</t>
+  </si>
+  <si>
+    <t>Dictionary update failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语法构建成功</t>
+  </si>
+  <si>
+    <t>Grammar build succeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前正在说话，音量大小</t>
+  </si>
+  <si>
+    <t>返回音频数据</t>
+  </si>
+  <si>
+    <t>Return audio data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结束说话</t>
+  </si>
+  <si>
+    <t>Stop speaking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始说话</t>
+  </si>
+  <si>
+    <t>Start speaking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>听写失败</t>
+  </si>
+  <si>
+    <t>Recognition failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取音频流失败</t>
+  </si>
+  <si>
+    <t>Failed to read the audio stream</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传热词失败</t>
+  </si>
+  <si>
+    <t>Failed to upload the hot words</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speaking, volumn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传联系人失败</t>
+  </si>
+  <si>
+    <t>Failed to upload contacts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>评测结束</t>
+  </si>
+  <si>
+    <t>Evaluation complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>请点击</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="Lucida Sans Typewriter"/>
+        <family val="3"/>
+      </rPr>
+      <t>“</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>开始评测</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="Lucida Sans Typewriter"/>
+        <family val="3"/>
+      </rPr>
+      <t>”</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按钮</t>
+    </r>
+  </si>
+  <si>
+    <t>Please click "Start evaluation" button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前音量</t>
+  </si>
+  <si>
+    <t>Current volumn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请朗读以上内容</t>
+  </si>
+  <si>
+    <t>Please read the content above</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解析结果为空</t>
+  </si>
+  <si>
+    <t>The result is empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>评测已停止</t>
+  </si>
+  <si>
+    <t>The evaluation had stopped</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>等待结果中</t>
+  </si>
+  <si>
+    <t>waiting for the result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请登录</t>
+  </si>
+  <si>
+    <t>Please login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载体验吧</t>
+  </si>
+  <si>
+    <t>to download and experience</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="Lucida Sans Typewriter"/>
+        <family val="3"/>
+      </rPr>
+      <t>IsvDemo</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>中哦，为了代码简洁，就不放在一起啦</t>
+    </r>
+  </si>
+  <si>
+    <t>Not supported yet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户名不能为空</t>
+  </si>
+  <si>
+    <t>Username shall not be empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不支持中文字符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Do not support Chinese characters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不能包含空格</t>
+  </si>
+  <si>
+    <t>Do not support spaces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>6-18</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个字母、数字或下划线的组合，以字母开头</t>
+    </r>
+  </si>
+  <si>
+    <t>6-18 characters, contains letter, digits, and underscore _, starts with letter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立刻体验语音听写</t>
+  </si>
+  <si>
+    <t>立刻体验语法识别</t>
+  </si>
+  <si>
+    <t>Grammar Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立刻体验语义理解</t>
+  </si>
+  <si>
+    <t>Semantic Understanding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立刻体验语音合成</t>
+  </si>
+  <si>
+    <t>Text to Speech</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automatic Speech Recognition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立刻体验语音评测</t>
+  </si>
+  <si>
+    <t>Speech evaluation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立刻体验语音唤醒</t>
+  </si>
+  <si>
+    <t>Voice wakeup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立刻体验声纹密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Voiceprint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语音合成失败</t>
+  </si>
+  <si>
+    <t>在线合成发音人选项</t>
+  </si>
+  <si>
+    <t>TTS failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TTS speaker options</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始播放</t>
+  </si>
+  <si>
+    <t>Start playing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂停播放</t>
+  </si>
+  <si>
+    <t>Pause playing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>继续播放</t>
+  </si>
+  <si>
+    <t>Resume playing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>播放完成</t>
+  </si>
+  <si>
+    <t>Playing complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合肥明天的天气怎么样?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the weather like tomorrow in San Francisco?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语义理解失败</t>
+  </si>
+  <si>
+    <t>停止录音</t>
+  </si>
+  <si>
+    <t>Stop recording</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Semantic Understanding failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>停止语义理解</t>
+  </si>
+  <si>
+    <t>Stop semantic understanding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消语义理解</t>
+  </si>
+  <si>
+    <t>Cancel semantic understanding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>识别结果不正确</t>
+  </si>
+  <si>
+    <t>Incorrect recognition result</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -364,7 +873,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +887,30 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF008000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF008000"/>
+      <name val="Lucida Sans Typewriter"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF008000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -400,8 +933,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -706,16 +1245,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.5" customWidth="1"/>
-    <col min="2" max="2" width="54.625" customWidth="1"/>
+    <col min="1" max="1" width="55.625" customWidth="1"/>
+    <col min="2" max="2" width="81.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -918,7 +1457,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -926,7 +1465,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -1060,6 +1599,470 @@
       </c>
       <c r="B43" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A44" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A49" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A56" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A57" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A58" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A59" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A60" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A61" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A62" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A63" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A64" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A65" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A66" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A67" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A68" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A69" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A70" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A71" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A73" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A74" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A75" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A76" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A77" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A78" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A79" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A80" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A81" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A82" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B82" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A83" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A84" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B84" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A85" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B85" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A86" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B86" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A87" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B87" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A88" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A89" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B89" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A90" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B90" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A91" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B91" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A92" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B92" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A93" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B93" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A94" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B94" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A95" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B95" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A96" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A97" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A98" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B98" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A99" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B99" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A100" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B100" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.15">
+      <c r="A101" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B101" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>